<commit_message>
szacowanie czy starczy nam gotówki
</commit_message>
<xml_diff>
--- a/plan/WyborKredytu.xlsx
+++ b/plan/WyborKredytu.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
   <si>
     <t>EB</t>
   </si>
@@ -264,19 +264,59 @@
   <si>
     <t>80pln - wszystko, tylko do sprawdzenia, 
 czy jest kwota w PLN</t>
+  </si>
+  <si>
+    <t>na Progresie Słonka</t>
+  </si>
+  <si>
+    <t>z Tynki</t>
+  </si>
+  <si>
+    <t>na Progresie wspólnym</t>
+  </si>
+  <si>
+    <t>ze Świdnicy</t>
+  </si>
+  <si>
+    <t>od Borego</t>
+  </si>
+  <si>
+    <t>RAZEM</t>
+  </si>
+  <si>
+    <t>Gotówka posiadana</t>
+  </si>
+  <si>
+    <t>Planowane wydatki</t>
+  </si>
+  <si>
+    <t>wynagrodzenie dla Nowaka</t>
+  </si>
+  <si>
+    <t>środki potrzebne na zakup euro</t>
+  </si>
+  <si>
+    <t>inne</t>
+  </si>
+  <si>
+    <t>na beton (wg oferty Manexu)</t>
+  </si>
+  <si>
+    <t>środki potrzebne na zakup euro (wartość z komórki A14)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;zł&quot;;[Red]\-#,##0.00\ &quot;zł&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +358,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -575,7 +623,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -683,6 +731,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1753,134 +1809,375 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="111.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="42" t="s">
         <v>69</v>
       </c>
       <c r="B1" s="41"/>
     </row>
-    <row r="3" spans="1:2" ht="64.5" customHeight="1">
+    <row r="3" spans="1:3" ht="64.5" customHeight="1">
       <c r="B3" s="38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="C4" s="46"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="40">
         <v>62800</v>
       </c>
       <c r="B5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="9.75" customHeight="1">
+      <c r="C5" s="44"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="40"/>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="44"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="39">
         <v>113000</v>
       </c>
       <c r="B7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="44"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="40">
         <f>A7/A11</f>
-        <v>25917.431192660548</v>
+        <v>25681.81818181818</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="6.75" customHeight="1">
+      <c r="C8" s="44"/>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="40"/>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="44"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="39">
-        <v>4.3499999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="45"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
       <c r="A11" s="39">
-        <v>4.3600000000000003</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="9" customHeight="1"/>
-    <row r="13" spans="1:2">
+      <c r="C11" s="46"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" s="44"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="40">
         <f>A5-A8</f>
-        <v>36882.568807339456</v>
+        <v>37118.181818181823</v>
       </c>
       <c r="B13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="44"/>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="39">
         <f>A13*A10</f>
-        <v>160439.17431192662</v>
+        <v>159608.18181818182</v>
       </c>
       <c r="B14" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="12" customHeight="1">
+      <c r="C14" s="44"/>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="39"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" s="41" t="s">
+      <c r="C15" s="44"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="46"/>
+      <c r="B16" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="44"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="44">
+        <v>30500</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="44"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="44">
+        <v>20900</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="44"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="44">
+        <v>10000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="44"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="44">
+        <v>10000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="44"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="44">
+        <v>110000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="44"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="45">
+        <f>SUM(A17:A21)</f>
+        <v>181400</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="44"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="C23" s="44"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75">
+      <c r="A24" s="46"/>
+      <c r="B24" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="44"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="44">
+        <v>8000</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="44"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="44">
+        <v>10000</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="44"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="44">
+        <f>A14</f>
+        <v>159608.18181818182</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="44"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="44"/>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="44"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="45">
+        <f>SUM(A25:A28)</f>
+        <v>177608.18181818182</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="44"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="45"/>
+      <c r="C30" s="44"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="45"/>
+      <c r="C31" s="44"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" s="41" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" ht="45">
-      <c r="B17" s="38" t="s">
+      <c r="C32" s="45"/>
+    </row>
+    <row r="33" spans="2:3" ht="60.75">
+      <c r="B33" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C33" s="43" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="30.75">
-      <c r="B18" s="38" t="s">
+    <row r="34" spans="2:3" ht="45.75">
+      <c r="B34" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C34" s="43" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="15.75">
-      <c r="B19" s="38" t="s">
+    <row r="35" spans="2:3" ht="15.75">
+      <c r="B35" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15.75">
-      <c r="B20" s="38" t="s">
+    <row r="36" spans="2:3" ht="15.75">
+      <c r="B36" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C36" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="15.75">
+      <c r="B39" s="46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="44">
+        <v>29000</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="44">
+        <v>21000</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="44">
+        <v>10000</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="44">
+        <v>10000</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="44">
+        <v>110000</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="45">
+        <f>SUM(B40:B44)</f>
+        <v>180000</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15.75">
+      <c r="B47" s="46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="44">
+        <v>8000</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="44">
+        <v>10000</v>
+      </c>
+      <c r="C49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="44">
+        <f>A14</f>
+        <v>159608.18181818182</v>
+      </c>
+      <c r="C50" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="44"/>
+      <c r="C51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="45">
+        <f>SUM(B48:B51)</f>
+        <v>177608.18181818182</v>
+      </c>
+      <c r="C52" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>